<commit_message>
handle empty multiform sheet and add resistance to cell values
</commit_message>
<xml_diff>
--- a/api/tests/acceptance/scripts/target-profile-migrations/migration-test-multiform_2.xlsx
+++ b/api/tests/acceptance/scripts/target-profile-migrations/migration-test-multiform_2.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="2007" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="2008" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="2010" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="2012" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
   <si>
     <t xml:space="preserve">id de sujet</t>
   </si>
@@ -43,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aucune instruction</t>
   </si>
 </sst>
 </file>
@@ -161,7 +165,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
   </cols>
@@ -220,7 +224,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -280,11 +284,11 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="12.63"/>
@@ -328,6 +332,35 @@
       </c>
       <c r="B5" s="2" t="n">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve handle of empty multiform file
</commit_message>
<xml_diff>
--- a/api/tests/acceptance/scripts/target-profile-migrations/migration-test-multiform_2.xlsx
+++ b/api/tests/acceptance/scripts/target-profile-migrations/migration-test-multiform_2.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="2007" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="2008" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="2010" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="2012" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="2013" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t xml:space="preserve">id de sujet</t>
   </si>
@@ -165,7 +166,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
   </cols>
@@ -224,7 +225,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -288,7 +289,7 @@
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="12.63"/>
@@ -352,11 +353,40 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>